<commit_message>
27 June 2018 get element with datatable
</commit_message>
<xml_diff>
--- a/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
+++ b/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>URL:</t>
   </si>
   <si>
-    <t>https://goolge.com</t>
-  </si>
-  <si>
     <t>Element Name:</t>
   </si>
   <si>
@@ -44,10 +41,19 @@
     <t>Element Value:</t>
   </si>
   <si>
-    <t>Input-search</t>
-  </si>
-  <si>
     <t>Data:</t>
+  </si>
+  <si>
+    <t>https://google.com.vn</t>
+  </si>
+  <si>
+    <t>lst-ib</t>
+  </si>
+  <si>
+    <t>btnK</t>
+  </si>
+  <si>
+    <t>search-name</t>
   </si>
 </sst>
 </file>
@@ -62,8 +68,9 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -86,14 +93,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,45 +378,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push code flight form
</commit_message>
<xml_diff>
--- a/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
+++ b/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>URL:</t>
   </si>
@@ -35,25 +35,55 @@
     <t>Element Name:</t>
   </si>
   <si>
-    <t>Search-txt-id</t>
-  </si>
-  <si>
     <t>Element Value:</t>
   </si>
   <si>
     <t>Data:</t>
   </si>
   <si>
-    <t>https://google.com.vn</t>
-  </si>
-  <si>
-    <t>lst-ib</t>
-  </si>
-  <si>
-    <t>btnK</t>
-  </si>
-  <si>
-    <t>search-name</t>
+    <t>tab-flight-tab-hp</t>
+  </si>
+  <si>
+    <t>tab-flight-btn-id</t>
+  </si>
+  <si>
+    <t>flight-origin-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-destination-hp-flight</t>
+  </si>
+  <si>
+    <t>flignt-origin-txt-id</t>
+  </si>
+  <si>
+    <t>flight-destination-txt-id</t>
+  </si>
+  <si>
+    <t>flight-departing-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-departing-txt-id</t>
+  </si>
+  <si>
+    <t>https://www.expedia.com/</t>
+  </si>
+  <si>
+    <t>gcw-submit</t>
+  </si>
+  <si>
+    <t>search-btn-class</t>
+  </si>
+  <si>
+    <t>flight-type-roundtrip-label-hp-flight</t>
+  </si>
+  <si>
+    <t>roundtrip-btn-id</t>
+  </si>
+  <si>
+    <t>flight-add-hotel-checkbox-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-add-hotel-ckb-id</t>
   </si>
 </sst>
 </file>
@@ -378,57 +408,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" display="https://google.com.vn"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
flight all form with input into checkin checkout
</commit_message>
<xml_diff>
--- a/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
+++ b/PhuongTran_Auto_Training/src/test/resources/DataIn/Elements.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>URL:</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>flight-add-hotel-ckb-id</t>
+  </si>
+  <si>
+    <t>flight-hotel-checkin-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-returning-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-returning-txt-id</t>
+  </si>
+  <si>
+    <t>flight-hotel-checkin-txt-id</t>
+  </si>
+  <si>
+    <t>flight-hotel-checkout-hp-flight</t>
+  </si>
+  <si>
+    <t>flight-hotel-checkout-txt-id</t>
+  </si>
+  <si>
+    <t>search-auto-id</t>
+  </si>
+  <si>
+    <t>aria-option-0</t>
   </si>
 </sst>
 </file>
@@ -408,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -421,12 +445,15 @@
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +462,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -452,16 +479,28 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -478,16 +517,28 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
         <v>13</v>
       </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>